<commit_message>
Se actualiza la base de datos de la rifa
</commit_message>
<xml_diff>
--- a/Patrocinio/Base de datos rifa.xlsx
+++ b/Patrocinio/Base de datos rifa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\entre\Desktop\FTC-Into_The_Deep\Patrocinio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4898DFF6-5CAE-479A-A58A-8B5CDB53D60B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2602EBF9-1F88-4EDC-8DB4-E4F7E33B77E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF5028DD-20EB-4666-BBAC-071ABD5BA7A7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="92">
   <si>
     <t>Y</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Diana Yate</t>
   </si>
   <si>
-    <t xml:space="preserve"> 310 391 5617</t>
-  </si>
-  <si>
     <t>315 378 0788</t>
   </si>
   <si>
@@ -192,6 +189,129 @@
   </si>
   <si>
     <t>Cristian Gamboa</t>
+  </si>
+  <si>
+    <t>Juan Emilio Mojica</t>
+  </si>
+  <si>
+    <t>310 391 5617</t>
+  </si>
+  <si>
+    <t>320 342 1617</t>
+  </si>
+  <si>
+    <t>304 325 9904</t>
+  </si>
+  <si>
+    <t>310 689 1989</t>
+  </si>
+  <si>
+    <t>310 775 4449</t>
+  </si>
+  <si>
+    <t>321 498 4677</t>
+  </si>
+  <si>
+    <t>318 411 3675</t>
+  </si>
+  <si>
+    <t>318 389 1142</t>
+  </si>
+  <si>
+    <t>300 557 4675</t>
+  </si>
+  <si>
+    <t>320 854 5733</t>
+  </si>
+  <si>
+    <t>221 3915</t>
+  </si>
+  <si>
+    <t>300 316 8624</t>
+  </si>
+  <si>
+    <t>318 243 2382</t>
+  </si>
+  <si>
+    <t>321 461 3347</t>
+  </si>
+  <si>
+    <t>317 331 9839</t>
+  </si>
+  <si>
+    <t>302 465 7363</t>
+  </si>
+  <si>
+    <t>314 323 7124</t>
+  </si>
+  <si>
+    <t>300 783 6077</t>
+  </si>
+  <si>
+    <t>315 687 4584</t>
+  </si>
+  <si>
+    <t>320 491 1463</t>
+  </si>
+  <si>
+    <t>302 528 6387</t>
+  </si>
+  <si>
+    <t>313 890 6050</t>
+  </si>
+  <si>
+    <t>313 412 7396</t>
+  </si>
+  <si>
+    <t>318 411 36375</t>
+  </si>
+  <si>
+    <t>Nicolás Rodríguez</t>
+  </si>
+  <si>
+    <t>Alejandro Huerfano</t>
+  </si>
+  <si>
+    <t>Nicolás Orjuela</t>
+  </si>
+  <si>
+    <t>Olga Herrera</t>
+  </si>
+  <si>
+    <t>Helber Berdugo</t>
+  </si>
+  <si>
+    <t>Pilar Quiñones</t>
+  </si>
+  <si>
+    <t>Germán Castro</t>
+  </si>
+  <si>
+    <t>Lorenzo Hurtado</t>
+  </si>
+  <si>
+    <t>Jairo Mojica</t>
+  </si>
+  <si>
+    <t>311 380 2673</t>
+  </si>
+  <si>
+    <t>300 539 8816</t>
+  </si>
+  <si>
+    <t>Martín Niño</t>
+  </si>
+  <si>
+    <t>319 654 6661</t>
+  </si>
+  <si>
+    <t>221 2915</t>
+  </si>
+  <si>
+    <t>316 834 8729</t>
+  </si>
+  <si>
+    <t>317 678 6506</t>
   </si>
 </sst>
 </file>
@@ -237,16 +357,16 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,8 +704,8 @@
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,7 +722,7 @@
       <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -616,7 +736,7 @@
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -644,7 +764,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -683,7 +803,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -713,7 +833,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -728,7 +848,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
@@ -746,7 +866,7 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
@@ -757,11 +877,11 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>25</v>
+      <c r="B12" t="s">
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -772,8 +892,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>23</v>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -784,8 +907,11 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>26</v>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -796,8 +922,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>22</v>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
       </c>
       <c r="D15" t="s">
         <v>0</v>
@@ -808,7 +937,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" t="s">
         <v>3</v>
       </c>
       <c r="D16" t="s">
@@ -820,8 +949,11 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>27</v>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
@@ -832,8 +964,11 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>28</v>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
@@ -844,7 +979,7 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" t="s">
         <v>3</v>
       </c>
       <c r="D19" t="s">
@@ -856,8 +991,11 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" t="s">
         <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
       </c>
       <c r="D20" t="s">
         <v>0</v>
@@ -868,8 +1006,14 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>29</v>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -877,8 +1021,11 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>30</v>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -886,8 +1033,14 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>31</v>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -895,8 +1048,14 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>29</v>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -904,8 +1063,14 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>32</v>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -913,8 +1078,14 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>23</v>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -922,8 +1093,14 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" t="s">
         <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -931,8 +1108,14 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>33</v>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -940,8 +1123,14 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>34</v>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -949,8 +1138,14 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>35</v>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -958,8 +1153,11 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>21</v>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -967,509 +1165,1019 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B33" s="4" t="s">
+      <c r="C34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B35" s="4" t="s">
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="B36" s="4" t="s">
+      <c r="C36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <f t="shared" si="0"/>
+      <c r="C38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" t="s">
+        <v>58</v>
+      </c>
+      <c r="D45" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>31</v>
+      </c>
+      <c r="C46" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" t="s">
+        <v>58</v>
+      </c>
+      <c r="D47" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" t="s">
+        <v>58</v>
+      </c>
+      <c r="D48" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" t="s">
+        <v>68</v>
+      </c>
+      <c r="D49" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" t="s">
+        <v>58</v>
+      </c>
+      <c r="D50" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" t="s">
+        <v>69</v>
+      </c>
+      <c r="D51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" t="s">
+        <v>72</v>
+      </c>
+      <c r="D55" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>48</v>
+      </c>
+      <c r="C57" t="s">
+        <v>73</v>
+      </c>
+      <c r="D57" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>38</v>
+      </c>
+      <c r="C58" t="s">
+        <v>64</v>
+      </c>
+      <c r="D58" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59" t="s">
+        <v>58</v>
+      </c>
+      <c r="D59" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>49</v>
+      </c>
+      <c r="D60" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>50</v>
+      </c>
+      <c r="C61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D61" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>40</v>
+      </c>
+      <c r="C63" t="s">
+        <v>75</v>
+      </c>
+      <c r="D63" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>23</v>
+      </c>
+      <c r="C64" t="s">
+        <v>53</v>
+      </c>
+      <c r="D64" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>31</v>
+      </c>
+      <c r="C65" t="s">
+        <v>58</v>
+      </c>
+      <c r="D65" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>76</v>
+      </c>
+      <c r="C66" t="s">
+        <v>85</v>
+      </c>
+      <c r="D66" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64">
-        <f t="shared" si="0"/>
+      <c r="C67" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D67" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <f t="shared" ref="A68:A101" si="1">SUM(A67+1)</f>
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>77</v>
+      </c>
+      <c r="D68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>37</v>
+      </c>
+      <c r="C69" t="s">
+        <v>63</v>
+      </c>
+      <c r="D69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>35</v>
+      </c>
+      <c r="C70" t="s">
+        <v>62</v>
+      </c>
+      <c r="D70" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>40</v>
+      </c>
+      <c r="C71" t="s">
+        <v>58</v>
+      </c>
+      <c r="D71" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>40</v>
+      </c>
+      <c r="C72" t="s">
+        <v>58</v>
+      </c>
+      <c r="D72" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>2</v>
+      </c>
+      <c r="C73" t="s">
+        <v>11</v>
+      </c>
+      <c r="D73" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>78</v>
+      </c>
+      <c r="D74" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>40</v>
+      </c>
+      <c r="C75" t="s">
+        <v>58</v>
+      </c>
+      <c r="D75" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>20</v>
+      </c>
+      <c r="D76" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>79</v>
+      </c>
+      <c r="C77" t="s">
+        <v>64</v>
+      </c>
+      <c r="D77" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>31</v>
+      </c>
+      <c r="C78" t="s">
+        <v>58</v>
+      </c>
+      <c r="D78" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>80</v>
+      </c>
+      <c r="C79" t="s">
+        <v>86</v>
+      </c>
+      <c r="D79" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>78</v>
+      </c>
+      <c r="D80" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>40</v>
+      </c>
+      <c r="C81" t="s">
+        <v>58</v>
+      </c>
+      <c r="D81" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>87</v>
+      </c>
+      <c r="C82" t="s">
+        <v>88</v>
+      </c>
+      <c r="D82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>79</v>
+      </c>
+      <c r="C83" t="s">
+        <v>64</v>
+      </c>
+      <c r="D83" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>81</v>
+      </c>
+      <c r="C84" t="s">
+        <v>10</v>
+      </c>
+      <c r="D84" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>35</v>
+      </c>
+      <c r="C85" t="s">
+        <v>89</v>
+      </c>
+      <c r="D85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>38</v>
+      </c>
+      <c r="C86" t="s">
+        <v>64</v>
+      </c>
+      <c r="D86" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87">
-        <f t="shared" si="1"/>
+        <f>SUM(A86+1)</f>
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C87" t="s">
+        <v>58</v>
+      </c>
+      <c r="D87" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88">
-        <f t="shared" si="1"/>
+        <f>SUM(A87+1)</f>
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>82</v>
+      </c>
+      <c r="C88" t="s">
+        <v>90</v>
+      </c>
+      <c r="D88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
+        <v>40</v>
+      </c>
+      <c r="C89" t="s">
+        <v>58</v>
+      </c>
+      <c r="D89" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>83</v>
+      </c>
+      <c r="C90" t="s">
+        <v>91</v>
+      </c>
+      <c r="D90" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
+        <v>40</v>
+      </c>
+      <c r="C91" t="s">
+        <v>58</v>
+      </c>
+      <c r="D91" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
+        <v>31</v>
+      </c>
+      <c r="C92" t="s">
+        <v>58</v>
+      </c>
+      <c r="D92" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
+        <v>40</v>
+      </c>
+      <c r="C93" t="s">
+        <v>58</v>
+      </c>
+      <c r="D93" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
+        <v>77</v>
+      </c>
+      <c r="D94" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>31</v>
+      </c>
+      <c r="C95" t="s">
+        <v>58</v>
+      </c>
+      <c r="D95" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>49</v>
+      </c>
+      <c r="D96" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>46</v>
+      </c>
+      <c r="C97" t="s">
+        <v>71</v>
+      </c>
+      <c r="D97" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>40</v>
+      </c>
+      <c r="C98" t="s">
+        <v>58</v>
+      </c>
+      <c r="D98" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
+        <v>78</v>
+      </c>
+      <c r="D99" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>84</v>
+      </c>
+      <c r="C100" t="s">
+        <v>57</v>
+      </c>
+      <c r="D100" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
         <f t="shared" si="1"/>
         <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>51</v>
+      </c>
+      <c r="C101" t="s">
+        <v>57</v>
+      </c>
+      <c r="D101" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>